<commit_message>
Update Hardwarestruktur und Testprotokoll.xlsx
</commit_message>
<xml_diff>
--- a/Dokumente/Hardwarestruktur und Testprotokoll.xlsx
+++ b/Dokumente/Hardwarestruktur und Testprotokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\uC_Board\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660F91A4-17A6-4D5D-B84A-7CF3E7C8BD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734B5BB8-9C92-4521-A412-27D30346E604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,9 +265,6 @@
     <t>S12</t>
   </si>
   <si>
-    <t>Codebezeichner</t>
-  </si>
-  <si>
     <t>Signalbeschreibung</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>Unterschrift:</t>
+  </si>
+  <si>
+    <t>Codebezeichner (Variabelname)</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1622,79 +1622,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1719,31 +1647,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1787,48 +1691,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="39" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="81" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1903,10 +1770,133 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="81" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2290,7 +2280,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -2304,525 +2294,525 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="E1" s="97" t="s">
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="E1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
     </row>
     <row r="2" spans="1:7" ht="20.25">
-      <c r="A2" s="95"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="96"/>
+      <c r="A2" s="63"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:7" ht="20.25">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="97" t="s">
+      <c r="B3" s="132"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="174"/>
-      <c r="G3" s="174"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="E4" s="98"/>
+      <c r="E4" s="66"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="133" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="133"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="117"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="97" t="s">
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="66"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="174"/>
-      <c r="G5" s="174"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="98"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
     </row>
     <row r="8" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="134" t="s">
+      <c r="A9" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="138"/>
+      <c r="G9" s="91"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A10" s="139" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="140" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="140" t="s">
+      <c r="A10" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="93" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="140" t="s">
+      <c r="D10" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="140" t="s">
+      <c r="E10" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="140" t="s">
+      <c r="G10" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="141" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="11" spans="1:7" ht="15">
-      <c r="A11" s="102">
+      <c r="A11" s="70">
         <v>0</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="104">
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="72">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15">
-      <c r="A12" s="105">
+      <c r="A12" s="73">
         <v>1</v>
       </c>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="175"/>
-      <c r="F12" s="175"/>
-      <c r="G12" s="107">
+      <c r="D12" s="74"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
+      <c r="G12" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15">
-      <c r="A13" s="99">
+      <c r="A13" s="67">
         <v>2</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="100" t="s">
+      <c r="C13" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="104">
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="72">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15">
-      <c r="A14" s="105">
+      <c r="A14" s="73">
         <v>3</v>
       </c>
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="106" t="s">
+      <c r="C14" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="106"/>
-      <c r="E14" s="175"/>
-      <c r="F14" s="175"/>
-      <c r="G14" s="107">
+      <c r="D14" s="74"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="75">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15">
-      <c r="A15" s="99">
+      <c r="A15" s="67">
         <v>4</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="100" t="s">
+      <c r="C15" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103"/>
-      <c r="G15" s="104">
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15">
-      <c r="A16" s="105">
+      <c r="A16" s="73">
         <v>5</v>
       </c>
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="C16" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="106"/>
-      <c r="E16" s="175"/>
-      <c r="F16" s="175"/>
-      <c r="G16" s="107">
+      <c r="D16" s="74"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="75">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15">
-      <c r="A17" s="99">
+      <c r="A17" s="67">
         <v>6</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="100" t="s">
+      <c r="C17" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="103"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="104">
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="72">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A18" s="142">
+      <c r="A18" s="95">
         <v>7</v>
       </c>
-      <c r="B18" s="143" t="s">
+      <c r="B18" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="143" t="s">
+      <c r="C18" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="143"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="144">
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="97">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="20" spans="1:7" ht="15.75">
-      <c r="A20" s="134" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="135"/>
-      <c r="C20" s="136"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="137"/>
-      <c r="F20" s="137" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="138"/>
+      <c r="A20" s="87" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="91"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A21" s="139" t="s">
+      <c r="A21" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="93" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="93" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="94" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15">
+      <c r="A22" s="70">
+        <v>0</v>
+      </c>
+      <c r="B22" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="140" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="140" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="140" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="140" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="140" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="141" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15">
-      <c r="A22" s="102">
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="72">
         <v>0</v>
       </c>
-      <c r="B22" s="103" t="s">
+    </row>
+    <row r="23" spans="1:7" ht="15">
+      <c r="A23" s="73">
+        <v>1</v>
+      </c>
+      <c r="B23" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="103" t="s">
+      <c r="C23" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15">
-      <c r="A23" s="105">
+      <c r="D23" s="74"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="75">
         <v>1</v>
       </c>
-      <c r="B23" s="106" t="s">
+    </row>
+    <row r="24" spans="1:7" ht="15">
+      <c r="A24" s="67">
+        <v>6</v>
+      </c>
+      <c r="B24" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="106" t="s">
+      <c r="C24" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="106"/>
-      <c r="E23" s="175"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15">
-      <c r="A24" s="99">
+      <c r="D24" s="68"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="69">
         <v>6</v>
       </c>
-      <c r="B24" s="100" t="s">
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A25" s="95">
+        <v>7</v>
+      </c>
+      <c r="B25" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C25" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="100"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="101">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A25" s="142">
-        <v>7</v>
-      </c>
-      <c r="B25" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="143" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="143"/>
-      <c r="E25" s="143"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="144">
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="97">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="27" spans="1:7" ht="15.75">
-      <c r="A27" s="145" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="136"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="137"/>
-      <c r="F27" s="137" t="s">
+      <c r="A27" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="138"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="91"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A28" s="139" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="140" t="s">
+      <c r="A28" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="93" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="93" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="94" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15">
+      <c r="A29" s="70">
+        <v>0</v>
+      </c>
+      <c r="B29" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="140" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="140" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="140" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="140" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="141" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15">
-      <c r="A29" s="102">
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="72">
         <v>0</v>
       </c>
-      <c r="B29" s="103" t="s">
+    </row>
+    <row r="30" spans="1:7" ht="15">
+      <c r="A30" s="73">
+        <v>1</v>
+      </c>
+      <c r="B30" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="103" t="s">
+      <c r="C30" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="103"/>
-      <c r="E29" s="103"/>
-      <c r="F29" s="103"/>
-      <c r="G29" s="104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15">
-      <c r="A30" s="105">
+      <c r="D30" s="74"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="75">
         <v>1</v>
       </c>
-      <c r="B30" s="106" t="s">
+    </row>
+    <row r="31" spans="1:7" ht="15">
+      <c r="A31" s="67">
+        <v>2</v>
+      </c>
+      <c r="B31" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="106" t="s">
+      <c r="C31" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="106"/>
-      <c r="E30" s="175"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15">
-      <c r="A31" s="99">
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="72">
         <v>2</v>
       </c>
-      <c r="B31" s="100" t="s">
+    </row>
+    <row r="32" spans="1:7" ht="15">
+      <c r="A32" s="73">
+        <v>3</v>
+      </c>
+      <c r="B32" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="100" t="s">
+      <c r="C32" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="104">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15">
-      <c r="A32" s="105">
+      <c r="D32" s="74"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="75">
         <v>3</v>
       </c>
-      <c r="B32" s="106" t="s">
+    </row>
+    <row r="33" spans="1:7" ht="15">
+      <c r="A33" s="67">
+        <v>4</v>
+      </c>
+      <c r="B33" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="106" t="s">
+      <c r="C33" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="106"/>
-      <c r="E32" s="175"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="107">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15">
-      <c r="A33" s="99">
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="72">
         <v>4</v>
       </c>
-      <c r="B33" s="100" t="s">
+    </row>
+    <row r="34" spans="1:7" ht="15">
+      <c r="A34" s="73">
+        <v>5</v>
+      </c>
+      <c r="B34" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="100" t="s">
+      <c r="C34" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="103"/>
-      <c r="E33" s="103"/>
-      <c r="F33" s="103"/>
-      <c r="G33" s="104">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15">
-      <c r="A34" s="105">
+      <c r="D34" s="74"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="75">
         <v>5</v>
       </c>
-      <c r="B34" s="106" t="s">
+    </row>
+    <row r="35" spans="1:7" ht="15">
+      <c r="A35" s="67">
+        <v>6</v>
+      </c>
+      <c r="B35" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="106" t="s">
+      <c r="C35" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="106"/>
-      <c r="E34" s="175"/>
-      <c r="F34" s="106"/>
-      <c r="G34" s="107">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15">
-      <c r="A35" s="99">
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="72">
         <v>6</v>
       </c>
-      <c r="B35" s="100" t="s">
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A36" s="95">
+        <v>7</v>
+      </c>
+      <c r="B36" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="100" t="s">
+      <c r="C36" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="104">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="142">
-        <v>7</v>
-      </c>
-      <c r="B36" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="143" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="143"/>
-      <c r="E36" s="143"/>
-      <c r="F36" s="143"/>
-      <c r="G36" s="144">
+      <c r="D36" s="96"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="97">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2853,119 +2843,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="20.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="123" t="str">
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="134" t="str">
         <f>IF(Hardwarekonzept!C3="","",Hardwarekonzept!C3)</f>
         <v/>
       </c>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="122" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="122"/>
-      <c r="S1" s="122"/>
-      <c r="T1" s="122"/>
-      <c r="U1" s="122"/>
-      <c r="V1" s="122"/>
-      <c r="W1" s="123" t="str">
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="134"/>
+      <c r="P1" s="134"/>
+      <c r="Q1" s="135" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="135"/>
+      <c r="U1" s="135"/>
+      <c r="V1" s="135"/>
+      <c r="W1" s="134" t="str">
         <f>IF(Hardwarekonzept!C7="","",Hardwarekonzept!C7)</f>
         <v/>
       </c>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
-      <c r="Z1" s="123"/>
-      <c r="AA1" s="123"/>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="123"/>
+      <c r="X1" s="134"/>
+      <c r="Y1" s="134"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="134"/>
+      <c r="AB1" s="134"/>
+      <c r="AC1" s="134"/>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
-      <c r="AA2" s="125"/>
-      <c r="AB2" s="125"/>
-      <c r="AC2" s="125"/>
     </row>
     <row r="3" spans="1:30" ht="15">
-      <c r="A3" s="120"/>
-      <c r="B3" s="120"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="122" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="124" t="str">
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="134" t="str">
         <f>IF(Hardwarekonzept!C5="","",Hardwarekonzept!C5)</f>
         <v/>
       </c>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="124"/>
-      <c r="N3" s="124"/>
-      <c r="O3" s="124"/>
-      <c r="P3" s="124"/>
-      <c r="Q3" s="122" t="s">
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="122"/>
-      <c r="S3" s="122"/>
-      <c r="T3" s="122"/>
-      <c r="U3" s="122"/>
-      <c r="V3" s="122"/>
-      <c r="W3" s="124" t="str">
+      <c r="R3" s="135"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="134" t="str">
         <f>IF(Hardwarekonzept!F5="","",Hardwarekonzept!F5)</f>
         <v/>
       </c>
-      <c r="X3" s="124"/>
-      <c r="Y3" s="124"/>
-      <c r="Z3" s="124"/>
-      <c r="AA3" s="124"/>
-      <c r="AB3" s="124"/>
-      <c r="AC3" s="124"/>
+      <c r="X3" s="134"/>
+      <c r="Y3" s="134"/>
+      <c r="Z3" s="134"/>
+      <c r="AA3" s="134"/>
+      <c r="AB3" s="134"/>
+      <c r="AC3" s="134"/>
     </row>
     <row r="4" spans="1:30" ht="12" customHeight="1">
       <c r="A4" s="3"/>
@@ -2983,7 +2943,7 @@
       <c r="M4" s="44"/>
       <c r="N4" s="44"/>
       <c r="O4" s="44"/>
-      <c r="P4" s="126"/>
+      <c r="P4" s="45"/>
       <c r="Q4" s="44"/>
       <c r="R4" s="44"/>
       <c r="S4" s="44"/>
@@ -2995,84 +2955,82 @@
       <c r="Y4" s="44"/>
       <c r="Z4" s="44"/>
       <c r="AA4" s="44"/>
-      <c r="AB4" s="125"/>
-      <c r="AC4" s="125"/>
     </row>
     <row r="5" spans="1:30" ht="12" customHeight="1" thickBot="1">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
-      <c r="W5" s="69"/>
-      <c r="X5" s="69"/>
-      <c r="Y5" s="69"/>
-      <c r="Z5" s="69"/>
-      <c r="AA5" s="69"/>
-      <c r="AB5" s="69"/>
-      <c r="AC5" s="69"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
+      <c r="N5" s="143"/>
+      <c r="O5" s="143"/>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="143"/>
+      <c r="R5" s="143"/>
+      <c r="S5" s="143"/>
+      <c r="T5" s="143"/>
+      <c r="U5" s="143"/>
+      <c r="V5" s="143"/>
+      <c r="W5" s="143"/>
+      <c r="X5" s="143"/>
+      <c r="Y5" s="143"/>
+      <c r="Z5" s="143"/>
+      <c r="AA5" s="143"/>
+      <c r="AB5" s="143"/>
+      <c r="AC5" s="143"/>
     </row>
     <row r="6" spans="1:30" ht="17.25" customHeight="1">
       <c r="A6" s="28"/>
       <c r="B6" s="23"/>
       <c r="C6" s="24"/>
-      <c r="D6" s="51" t="str">
+      <c r="D6" s="147" t="str">
         <f>IF(Hardwarekonzept!G9="","Schalter (Port __)","Schalter (Port "&amp;Hardwarekonzept!G9&amp;")")</f>
         <v>Schalter (Port __)</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53" t="str">
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="164"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="164"/>
+      <c r="K6" s="164"/>
+      <c r="L6" s="165" t="str">
         <f>IF(Hardwarekonzept!G20="","Taster (Port __)","Taster (Port "&amp;Hardwarekonzept!G20&amp;")")</f>
         <v>Taster (Port __)</v>
       </c>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="55"/>
+      <c r="M6" s="166"/>
+      <c r="N6" s="166"/>
+      <c r="O6" s="167"/>
       <c r="P6" s="40" t="s">
         <v>10</v>
       </c>
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
-      <c r="S6" s="51" t="str">
+      <c r="S6" s="147" t="str">
         <f>IF(Hardwarekonzept!G27="","LED (Port __)","LED (Port "&amp;Hardwarekonzept!G27&amp;")")</f>
         <v>LED (Port __)</v>
       </c>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="56"/>
-      <c r="Z6" s="57"/>
-      <c r="AA6" s="65" t="s">
+      <c r="T6" s="148"/>
+      <c r="U6" s="148"/>
+      <c r="V6" s="148"/>
+      <c r="W6" s="148"/>
+      <c r="X6" s="148"/>
+      <c r="Y6" s="148"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="157" t="s">
         <v>9</v>
       </c>
-      <c r="AB6" s="66"/>
+      <c r="AB6" s="158"/>
       <c r="AC6" s="14"/>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1">
@@ -3084,71 +3042,71 @@
       <c r="D7" s="5">
         <v>7</v>
       </c>
-      <c r="E7" s="147">
+      <c r="E7" s="100">
         <v>6</v>
       </c>
       <c r="F7" s="5">
         <v>5</v>
       </c>
-      <c r="G7" s="147">
+      <c r="G7" s="100">
         <v>4</v>
       </c>
       <c r="H7" s="5">
         <v>3</v>
       </c>
-      <c r="I7" s="147">
+      <c r="I7" s="100">
         <v>2</v>
       </c>
       <c r="J7" s="20">
         <v>1</v>
       </c>
-      <c r="K7" s="154">
+      <c r="K7" s="107">
         <v>0</v>
       </c>
       <c r="L7" s="38">
         <v>7</v>
       </c>
-      <c r="M7" s="160">
+      <c r="M7" s="113">
         <v>6</v>
       </c>
       <c r="N7" s="21">
         <v>1</v>
       </c>
-      <c r="O7" s="162">
+      <c r="O7" s="115">
         <v>0</v>
       </c>
-      <c r="P7" s="60" t="s">
+      <c r="P7" s="152" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="62"/>
+      <c r="Q7" s="153"/>
+      <c r="R7" s="154"/>
       <c r="S7" s="5">
         <v>7</v>
       </c>
-      <c r="T7" s="147">
+      <c r="T7" s="100">
         <v>6</v>
       </c>
       <c r="U7" s="5">
         <v>5</v>
       </c>
-      <c r="V7" s="147">
+      <c r="V7" s="100">
         <v>4</v>
       </c>
       <c r="W7" s="5">
         <v>3</v>
       </c>
-      <c r="X7" s="147">
+      <c r="X7" s="100">
         <v>2</v>
       </c>
       <c r="Y7" s="5">
         <v>1</v>
       </c>
-      <c r="Z7" s="171">
+      <c r="Z7" s="124">
         <v>0</v>
       </c>
-      <c r="AA7" s="58"/>
-      <c r="AB7" s="59"/>
-      <c r="AC7" s="63" t="s">
+      <c r="AA7" s="150"/>
+      <c r="AB7" s="151"/>
+      <c r="AC7" s="155" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3159,93 +3117,93 @@
       <c r="B8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="112" t="s">
+      <c r="C8" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="113" t="str">
+      <c r="D8" s="81" t="str">
         <f>IF(Hardwarekonzept!F18="","",Hardwarekonzept!F18)</f>
         <v/>
       </c>
-      <c r="E8" s="148" t="str">
+      <c r="E8" s="101" t="str">
         <f>IF(Hardwarekonzept!F17="","",Hardwarekonzept!F17)</f>
         <v/>
       </c>
-      <c r="F8" s="113" t="str">
+      <c r="F8" s="81" t="str">
         <f>IF(Hardwarekonzept!F16="","",Hardwarekonzept!F16)</f>
         <v/>
       </c>
-      <c r="G8" s="148" t="str">
+      <c r="G8" s="101" t="str">
         <f>IF(Hardwarekonzept!F15="","",Hardwarekonzept!F15)</f>
         <v/>
       </c>
-      <c r="H8" s="113" t="str">
+      <c r="H8" s="81" t="str">
         <f>IF(Hardwarekonzept!F14="","",Hardwarekonzept!F14)</f>
         <v/>
       </c>
-      <c r="I8" s="148" t="str">
+      <c r="I8" s="101" t="str">
         <f>IF(Hardwarekonzept!F13="","",Hardwarekonzept!F13)</f>
         <v/>
       </c>
-      <c r="J8" s="113" t="str">
+      <c r="J8" s="81" t="str">
         <f>IF(Hardwarekonzept!F12="","",Hardwarekonzept!F12)</f>
         <v/>
       </c>
-      <c r="K8" s="155" t="str">
+      <c r="K8" s="108" t="str">
         <f>IF(Hardwarekonzept!F11="","",Hardwarekonzept!F11)</f>
         <v/>
       </c>
-      <c r="L8" s="114" t="str">
+      <c r="L8" s="82" t="str">
         <f>IF(Hardwarekonzept!F25="","",Hardwarekonzept!F25)</f>
         <v/>
       </c>
-      <c r="M8" s="161" t="str">
+      <c r="M8" s="114" t="str">
         <f>IF(Hardwarekonzept!F24="","",Hardwarekonzept!F24)</f>
         <v/>
       </c>
-      <c r="N8" s="115" t="str">
+      <c r="N8" s="83" t="str">
         <f>IF(Hardwarekonzept!F23="","",Hardwarekonzept!F23)</f>
         <v/>
       </c>
-      <c r="O8" s="163" t="str">
+      <c r="O8" s="116" t="str">
         <f>IF(Hardwarekonzept!F22="","",Hardwarekonzept!F22)</f>
         <v/>
       </c>
-      <c r="P8" s="67" t="s">
+      <c r="P8" s="159" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="109" t="s">
+      <c r="Q8" s="160"/>
+      <c r="R8" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="108" t="str">
+      <c r="S8" s="76" t="str">
         <f>IF(Hardwarekonzept!$F36="","",Hardwarekonzept!$F36)</f>
         <v/>
       </c>
-      <c r="T8" s="169" t="str">
+      <c r="T8" s="122" t="str">
         <f>IF(Hardwarekonzept!$F35="","",Hardwarekonzept!$F35)</f>
         <v/>
       </c>
-      <c r="U8" s="110" t="str">
+      <c r="U8" s="78" t="str">
         <f>IF(Hardwarekonzept!$F34="","",Hardwarekonzept!$F34)</f>
         <v/>
       </c>
-      <c r="V8" s="170" t="str">
+      <c r="V8" s="123" t="str">
         <f>IF(Hardwarekonzept!$F33="","",Hardwarekonzept!$F33)</f>
         <v/>
       </c>
-      <c r="W8" s="108" t="str">
+      <c r="W8" s="76" t="str">
         <f>IF(Hardwarekonzept!$F32="","",Hardwarekonzept!$F32)</f>
         <v/>
       </c>
-      <c r="X8" s="170" t="str">
+      <c r="X8" s="123" t="str">
         <f>IF(Hardwarekonzept!$F31="","",Hardwarekonzept!$F31)</f>
         <v/>
       </c>
-      <c r="Y8" s="111" t="str">
+      <c r="Y8" s="79" t="str">
         <f>IF(Hardwarekonzept!$F30="","",Hardwarekonzept!$F30)</f>
         <v/>
       </c>
-      <c r="Z8" s="172" t="str">
+      <c r="Z8" s="125" t="str">
         <f>IF(Hardwarekonzept!$F29="","",Hardwarekonzept!$F29)</f>
         <v/>
       </c>
@@ -3255,34 +3213,34 @@
       <c r="AB8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="AC8" s="64"/>
+      <c r="AC8" s="156"/>
     </row>
     <row r="9" spans="1:30" ht="0.75" customHeight="1" thickBot="1">
       <c r="A9" s="31"/>
       <c r="B9" s="27"/>
       <c r="C9" s="12"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="149"/>
+      <c r="E9" s="102"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="149"/>
+      <c r="G9" s="102"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="149"/>
+      <c r="I9" s="102"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="149"/>
+      <c r="K9" s="102"/>
       <c r="L9" s="41"/>
-      <c r="M9" s="149"/>
+      <c r="M9" s="102"/>
       <c r="N9" s="17"/>
-      <c r="O9" s="164"/>
+      <c r="O9" s="117"/>
       <c r="P9" s="22"/>
       <c r="R9" s="17"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="149"/>
+      <c r="T9" s="102"/>
       <c r="U9" s="10"/>
-      <c r="V9" s="149"/>
+      <c r="V9" s="102"/>
       <c r="W9" s="10"/>
-      <c r="X9" s="149"/>
+      <c r="X9" s="102"/>
       <c r="Y9" s="11"/>
-      <c r="Z9" s="173"/>
+      <c r="Z9" s="126"/>
       <c r="AA9" s="13"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="14"/>
@@ -3291,99 +3249,99 @@
       <c r="A10" s="32">
         <v>1</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="50"/>
+      <c r="B10" s="161"/>
+      <c r="C10" s="163"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="150"/>
+      <c r="E10" s="103"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="150"/>
+      <c r="G10" s="103"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="150"/>
+      <c r="I10" s="103"/>
       <c r="J10" s="16"/>
-      <c r="K10" s="156"/>
+      <c r="K10" s="109"/>
       <c r="L10" s="36"/>
-      <c r="M10" s="150"/>
+      <c r="M10" s="103"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="165"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="50"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="161"/>
+      <c r="Q10" s="162"/>
+      <c r="R10" s="163"/>
       <c r="S10" s="16"/>
-      <c r="T10" s="150"/>
+      <c r="T10" s="103"/>
       <c r="U10" s="16"/>
-      <c r="V10" s="150"/>
+      <c r="V10" s="103"/>
       <c r="W10" s="16"/>
-      <c r="X10" s="150"/>
+      <c r="X10" s="103"/>
       <c r="Y10" s="16"/>
-      <c r="Z10" s="165"/>
+      <c r="Z10" s="118"/>
       <c r="AA10" s="34"/>
       <c r="AB10" s="15"/>
       <c r="AC10" s="42"/>
       <c r="AD10" s="9"/>
     </row>
     <row r="11" spans="1:30" ht="42" customHeight="1">
-      <c r="A11" s="70">
+      <c r="A11" s="46">
         <v>2</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="151"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="151"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="151"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="157"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="151"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="166"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="92"/>
-      <c r="R11" s="91"/>
-      <c r="S11" s="71"/>
-      <c r="T11" s="151"/>
-      <c r="U11" s="71"/>
-      <c r="V11" s="151"/>
-      <c r="W11" s="71"/>
-      <c r="X11" s="151"/>
-      <c r="Y11" s="71"/>
-      <c r="Z11" s="166"/>
-      <c r="AA11" s="93"/>
-      <c r="AB11" s="94"/>
-      <c r="AC11" s="74"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="110"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="144"/>
+      <c r="Q11" s="146"/>
+      <c r="R11" s="145"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="104"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="104"/>
+      <c r="W11" s="47"/>
+      <c r="X11" s="104"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="119"/>
+      <c r="AA11" s="61"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="50"/>
       <c r="AD11" s="9"/>
     </row>
     <row r="12" spans="1:30" ht="42" customHeight="1">
       <c r="A12" s="33">
         <v>3</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="47"/>
+      <c r="B12" s="137"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="152"/>
+      <c r="E12" s="105"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="152"/>
+      <c r="G12" s="105"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="152"/>
+      <c r="I12" s="105"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="158"/>
+      <c r="K12" s="111"/>
       <c r="L12" s="37"/>
-      <c r="M12" s="152"/>
+      <c r="M12" s="105"/>
       <c r="N12" s="19"/>
-      <c r="O12" s="167"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="47"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="137"/>
+      <c r="Q12" s="138"/>
+      <c r="R12" s="139"/>
       <c r="S12" s="6"/>
-      <c r="T12" s="152"/>
+      <c r="T12" s="105"/>
       <c r="U12" s="6"/>
-      <c r="V12" s="152"/>
+      <c r="V12" s="105"/>
       <c r="W12" s="6"/>
-      <c r="X12" s="152"/>
+      <c r="X12" s="105"/>
       <c r="Y12" s="6"/>
-      <c r="Z12" s="167"/>
+      <c r="Z12" s="120"/>
       <c r="AA12" s="35"/>
       <c r="AB12" s="8"/>
       <c r="AC12" s="43"/>
@@ -3393,31 +3351,31 @@
       <c r="A13" s="33">
         <v>4</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="47"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="139"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="152"/>
+      <c r="E13" s="105"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="152"/>
+      <c r="G13" s="105"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="152"/>
+      <c r="I13" s="105"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="158"/>
+      <c r="K13" s="111"/>
       <c r="L13" s="37"/>
-      <c r="M13" s="152"/>
+      <c r="M13" s="105"/>
       <c r="N13" s="19"/>
-      <c r="O13" s="167"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="47"/>
+      <c r="O13" s="120"/>
+      <c r="P13" s="137"/>
+      <c r="Q13" s="138"/>
+      <c r="R13" s="139"/>
       <c r="S13" s="6"/>
-      <c r="T13" s="152"/>
+      <c r="T13" s="105"/>
       <c r="U13" s="6"/>
-      <c r="V13" s="152"/>
+      <c r="V13" s="105"/>
       <c r="W13" s="6"/>
-      <c r="X13" s="152"/>
+      <c r="X13" s="105"/>
       <c r="Y13" s="6"/>
-      <c r="Z13" s="167"/>
+      <c r="Z13" s="120"/>
       <c r="AA13" s="35"/>
       <c r="AB13" s="8"/>
       <c r="AC13" s="43"/>
@@ -3427,31 +3385,31 @@
       <c r="A14" s="33">
         <v>5</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="47"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="139"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="152"/>
+      <c r="E14" s="105"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="152"/>
+      <c r="G14" s="105"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="152"/>
+      <c r="I14" s="105"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="158"/>
+      <c r="K14" s="111"/>
       <c r="L14" s="37"/>
-      <c r="M14" s="152"/>
+      <c r="M14" s="105"/>
       <c r="N14" s="19"/>
-      <c r="O14" s="167"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="47"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="137"/>
+      <c r="Q14" s="138"/>
+      <c r="R14" s="139"/>
       <c r="S14" s="6"/>
-      <c r="T14" s="152"/>
+      <c r="T14" s="105"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="152"/>
+      <c r="V14" s="105"/>
       <c r="W14" s="6"/>
-      <c r="X14" s="152"/>
+      <c r="X14" s="105"/>
       <c r="Y14" s="6"/>
-      <c r="Z14" s="167"/>
+      <c r="Z14" s="120"/>
       <c r="AA14" s="35"/>
       <c r="AB14" s="8"/>
       <c r="AC14" s="43"/>
@@ -3461,31 +3419,31 @@
       <c r="A15" s="33">
         <v>6</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="47"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="139"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="152"/>
+      <c r="E15" s="105"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="152"/>
+      <c r="G15" s="105"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="152"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="158"/>
+      <c r="K15" s="111"/>
       <c r="L15" s="37"/>
-      <c r="M15" s="152"/>
+      <c r="M15" s="105"/>
       <c r="N15" s="19"/>
-      <c r="O15" s="167"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="47"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="137"/>
+      <c r="Q15" s="138"/>
+      <c r="R15" s="139"/>
       <c r="S15" s="6"/>
-      <c r="T15" s="152"/>
+      <c r="T15" s="105"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="152"/>
+      <c r="V15" s="105"/>
       <c r="W15" s="6"/>
-      <c r="X15" s="152"/>
+      <c r="X15" s="105"/>
       <c r="Y15" s="6"/>
-      <c r="Z15" s="167"/>
+      <c r="Z15" s="120"/>
       <c r="AA15" s="35"/>
       <c r="AB15" s="8"/>
       <c r="AC15" s="43"/>
@@ -3495,31 +3453,31 @@
       <c r="A16" s="33">
         <v>7</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="47"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="139"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="152"/>
+      <c r="E16" s="105"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="152"/>
+      <c r="G16" s="105"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="152"/>
+      <c r="I16" s="105"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="158"/>
+      <c r="K16" s="111"/>
       <c r="L16" s="37"/>
-      <c r="M16" s="152"/>
+      <c r="M16" s="105"/>
       <c r="N16" s="19"/>
-      <c r="O16" s="167"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="47"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="137"/>
+      <c r="Q16" s="138"/>
+      <c r="R16" s="139"/>
       <c r="S16" s="6"/>
-      <c r="T16" s="152"/>
+      <c r="T16" s="105"/>
       <c r="U16" s="6"/>
-      <c r="V16" s="152"/>
+      <c r="V16" s="105"/>
       <c r="W16" s="6"/>
-      <c r="X16" s="152"/>
+      <c r="X16" s="105"/>
       <c r="Y16" s="6"/>
-      <c r="Z16" s="167"/>
+      <c r="Z16" s="120"/>
       <c r="AA16" s="35"/>
       <c r="AB16" s="8"/>
       <c r="AC16" s="43"/>
@@ -3529,31 +3487,31 @@
       <c r="A17" s="33">
         <v>8</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="47"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="139"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="152"/>
+      <c r="E17" s="105"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="152"/>
+      <c r="G17" s="105"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="152"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="158"/>
+      <c r="K17" s="111"/>
       <c r="L17" s="37"/>
-      <c r="M17" s="152"/>
+      <c r="M17" s="105"/>
       <c r="N17" s="19"/>
-      <c r="O17" s="167"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="47"/>
+      <c r="O17" s="120"/>
+      <c r="P17" s="137"/>
+      <c r="Q17" s="138"/>
+      <c r="R17" s="139"/>
       <c r="S17" s="6"/>
-      <c r="T17" s="152"/>
+      <c r="T17" s="105"/>
       <c r="U17" s="6"/>
-      <c r="V17" s="152"/>
+      <c r="V17" s="105"/>
       <c r="W17" s="6"/>
-      <c r="X17" s="152"/>
+      <c r="X17" s="105"/>
       <c r="Y17" s="6"/>
-      <c r="Z17" s="167"/>
+      <c r="Z17" s="120"/>
       <c r="AA17" s="35"/>
       <c r="AB17" s="8"/>
       <c r="AC17" s="43"/>
@@ -3563,99 +3521,99 @@
       <c r="A18" s="33">
         <v>9</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="47"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="139"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="152"/>
+      <c r="E18" s="105"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="152"/>
+      <c r="G18" s="105"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="152"/>
+      <c r="I18" s="105"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="158"/>
+      <c r="K18" s="111"/>
       <c r="L18" s="37"/>
-      <c r="M18" s="152"/>
+      <c r="M18" s="105"/>
       <c r="N18" s="19"/>
-      <c r="O18" s="167"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="47"/>
+      <c r="O18" s="120"/>
+      <c r="P18" s="137"/>
+      <c r="Q18" s="138"/>
+      <c r="R18" s="139"/>
       <c r="S18" s="6"/>
-      <c r="T18" s="152"/>
+      <c r="T18" s="105"/>
       <c r="U18" s="6"/>
-      <c r="V18" s="152"/>
+      <c r="V18" s="105"/>
       <c r="W18" s="6"/>
-      <c r="X18" s="152"/>
+      <c r="X18" s="105"/>
       <c r="Y18" s="6"/>
-      <c r="Z18" s="167"/>
+      <c r="Z18" s="120"/>
       <c r="AA18" s="35"/>
       <c r="AB18" s="8"/>
       <c r="AC18" s="43"/>
       <c r="AD18" s="9"/>
     </row>
     <row r="19" spans="1:30" ht="42" customHeight="1">
-      <c r="A19" s="75">
+      <c r="A19" s="51">
         <v>10</v>
       </c>
-      <c r="B19" s="87"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="153"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="153"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="153"/>
-      <c r="J19" s="76"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="153"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="168"/>
-      <c r="P19" s="87"/>
-      <c r="Q19" s="89"/>
-      <c r="R19" s="88"/>
-      <c r="S19" s="76"/>
-      <c r="T19" s="153"/>
-      <c r="U19" s="76"/>
-      <c r="V19" s="153"/>
-      <c r="W19" s="76"/>
-      <c r="X19" s="153"/>
-      <c r="Y19" s="76"/>
-      <c r="Z19" s="168"/>
-      <c r="AA19" s="79"/>
-      <c r="AB19" s="80"/>
-      <c r="AC19" s="81"/>
+      <c r="B19" s="140"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="112"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="106"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="121"/>
+      <c r="P19" s="140"/>
+      <c r="Q19" s="142"/>
+      <c r="R19" s="141"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="106"/>
+      <c r="U19" s="52"/>
+      <c r="V19" s="106"/>
+      <c r="W19" s="52"/>
+      <c r="X19" s="106"/>
+      <c r="Y19" s="52"/>
+      <c r="Z19" s="121"/>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="56"/>
+      <c r="AC19" s="57"/>
       <c r="AD19" s="9"/>
     </row>
     <row r="20" spans="1:30" ht="42" customHeight="1">
       <c r="A20" s="33">
         <v>11</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="47"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="139"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="152"/>
+      <c r="E20" s="105"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="152"/>
+      <c r="G20" s="105"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="152"/>
+      <c r="I20" s="105"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="158"/>
+      <c r="K20" s="111"/>
       <c r="L20" s="37"/>
-      <c r="M20" s="152"/>
+      <c r="M20" s="105"/>
       <c r="N20" s="19"/>
-      <c r="O20" s="167"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="47"/>
+      <c r="O20" s="120"/>
+      <c r="P20" s="137"/>
+      <c r="Q20" s="138"/>
+      <c r="R20" s="139"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="152"/>
+      <c r="T20" s="105"/>
       <c r="U20" s="6"/>
-      <c r="V20" s="152"/>
+      <c r="V20" s="105"/>
       <c r="W20" s="6"/>
-      <c r="X20" s="152"/>
+      <c r="X20" s="105"/>
       <c r="Y20" s="6"/>
-      <c r="Z20" s="167"/>
+      <c r="Z20" s="120"/>
       <c r="AA20" s="35"/>
       <c r="AB20" s="8"/>
       <c r="AC20" s="43"/>
@@ -3665,65 +3623,65 @@
       <c r="A21" s="33">
         <v>12</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="47"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="139"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="152"/>
+      <c r="E21" s="105"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="152"/>
+      <c r="G21" s="105"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="152"/>
+      <c r="I21" s="105"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="158"/>
+      <c r="K21" s="111"/>
       <c r="L21" s="37"/>
-      <c r="M21" s="152"/>
+      <c r="M21" s="105"/>
       <c r="N21" s="19"/>
-      <c r="O21" s="167"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="47"/>
+      <c r="O21" s="120"/>
+      <c r="P21" s="137"/>
+      <c r="Q21" s="138"/>
+      <c r="R21" s="139"/>
       <c r="S21" s="6"/>
-      <c r="T21" s="152"/>
+      <c r="T21" s="105"/>
       <c r="U21" s="6"/>
-      <c r="V21" s="152"/>
+      <c r="V21" s="105"/>
       <c r="W21" s="6"/>
-      <c r="X21" s="152"/>
+      <c r="X21" s="105"/>
       <c r="Y21" s="6"/>
-      <c r="Z21" s="167"/>
+      <c r="Z21" s="120"/>
       <c r="AA21" s="35"/>
       <c r="AB21" s="8"/>
       <c r="AC21" s="43"/>
       <c r="AD21" s="9"/>
     </row>
     <row r="22" spans="1:30" ht="42" customHeight="1">
-      <c r="A22" s="75">
+      <c r="A22" s="51">
         <v>13</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="47"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="139"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="152"/>
+      <c r="E22" s="105"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="152"/>
+      <c r="G22" s="105"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="152"/>
+      <c r="I22" s="105"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="158"/>
+      <c r="K22" s="111"/>
       <c r="L22" s="37"/>
-      <c r="M22" s="152"/>
+      <c r="M22" s="105"/>
       <c r="N22" s="19"/>
-      <c r="O22" s="167"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="47"/>
+      <c r="O22" s="120"/>
+      <c r="P22" s="137"/>
+      <c r="Q22" s="138"/>
+      <c r="R22" s="139"/>
       <c r="S22" s="6"/>
-      <c r="T22" s="152"/>
+      <c r="T22" s="105"/>
       <c r="U22" s="6"/>
-      <c r="V22" s="152"/>
+      <c r="V22" s="105"/>
       <c r="W22" s="6"/>
-      <c r="X22" s="152"/>
+      <c r="X22" s="105"/>
       <c r="Y22" s="6"/>
-      <c r="Z22" s="167"/>
+      <c r="Z22" s="120"/>
       <c r="AA22" s="35"/>
       <c r="AB22" s="8"/>
       <c r="AC22" s="43"/>
@@ -3733,31 +3691,31 @@
       <c r="A23" s="33">
         <v>14</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="47"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="139"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="152"/>
+      <c r="E23" s="105"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="152"/>
+      <c r="G23" s="105"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="152"/>
+      <c r="I23" s="105"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="158"/>
+      <c r="K23" s="111"/>
       <c r="L23" s="37"/>
-      <c r="M23" s="152"/>
+      <c r="M23" s="105"/>
       <c r="N23" s="19"/>
-      <c r="O23" s="167"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="47"/>
+      <c r="O23" s="120"/>
+      <c r="P23" s="137"/>
+      <c r="Q23" s="138"/>
+      <c r="R23" s="139"/>
       <c r="S23" s="6"/>
-      <c r="T23" s="152"/>
+      <c r="T23" s="105"/>
       <c r="U23" s="6"/>
-      <c r="V23" s="152"/>
+      <c r="V23" s="105"/>
       <c r="W23" s="6"/>
-      <c r="X23" s="152"/>
+      <c r="X23" s="105"/>
       <c r="Y23" s="6"/>
-      <c r="Z23" s="167"/>
+      <c r="Z23" s="120"/>
       <c r="AA23" s="35"/>
       <c r="AB23" s="8"/>
       <c r="AC23" s="43"/>
@@ -3767,65 +3725,65 @@
       <c r="A24" s="33">
         <v>15</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="47"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="139"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="152"/>
+      <c r="E24" s="105"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="152"/>
+      <c r="G24" s="105"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="152"/>
+      <c r="I24" s="105"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="158"/>
+      <c r="K24" s="111"/>
       <c r="L24" s="37"/>
-      <c r="M24" s="152"/>
+      <c r="M24" s="105"/>
       <c r="N24" s="19"/>
-      <c r="O24" s="167"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="47"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="137"/>
+      <c r="Q24" s="138"/>
+      <c r="R24" s="139"/>
       <c r="S24" s="6"/>
-      <c r="T24" s="152"/>
+      <c r="T24" s="105"/>
       <c r="U24" s="6"/>
-      <c r="V24" s="152"/>
+      <c r="V24" s="105"/>
       <c r="W24" s="6"/>
-      <c r="X24" s="152"/>
+      <c r="X24" s="105"/>
       <c r="Y24" s="6"/>
-      <c r="Z24" s="167"/>
+      <c r="Z24" s="120"/>
       <c r="AA24" s="35"/>
       <c r="AB24" s="8"/>
       <c r="AC24" s="43"/>
       <c r="AD24" s="9"/>
     </row>
     <row r="25" spans="1:30" ht="42" customHeight="1">
-      <c r="A25" s="75">
+      <c r="A25" s="51">
         <v>16</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="47"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="139"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="152"/>
+      <c r="E25" s="105"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="152"/>
+      <c r="G25" s="105"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="152"/>
+      <c r="I25" s="105"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="158"/>
+      <c r="K25" s="111"/>
       <c r="L25" s="37"/>
-      <c r="M25" s="152"/>
+      <c r="M25" s="105"/>
       <c r="N25" s="19"/>
-      <c r="O25" s="167"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="47"/>
+      <c r="O25" s="120"/>
+      <c r="P25" s="137"/>
+      <c r="Q25" s="138"/>
+      <c r="R25" s="139"/>
       <c r="S25" s="6"/>
-      <c r="T25" s="152"/>
+      <c r="T25" s="105"/>
       <c r="U25" s="6"/>
-      <c r="V25" s="152"/>
+      <c r="V25" s="105"/>
       <c r="W25" s="6"/>
-      <c r="X25" s="152"/>
+      <c r="X25" s="105"/>
       <c r="Y25" s="6"/>
-      <c r="Z25" s="167"/>
+      <c r="Z25" s="120"/>
       <c r="AA25" s="35"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="43"/>
@@ -3835,31 +3793,31 @@
       <c r="A26" s="33">
         <v>17</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="47"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="139"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="152"/>
+      <c r="E26" s="105"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="152"/>
+      <c r="G26" s="105"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="152"/>
+      <c r="I26" s="105"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="158"/>
+      <c r="K26" s="111"/>
       <c r="L26" s="37"/>
-      <c r="M26" s="152"/>
+      <c r="M26" s="105"/>
       <c r="N26" s="19"/>
-      <c r="O26" s="167"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="47"/>
+      <c r="O26" s="120"/>
+      <c r="P26" s="137"/>
+      <c r="Q26" s="138"/>
+      <c r="R26" s="139"/>
       <c r="S26" s="6"/>
-      <c r="T26" s="152"/>
+      <c r="T26" s="105"/>
       <c r="U26" s="6"/>
-      <c r="V26" s="152"/>
+      <c r="V26" s="105"/>
       <c r="W26" s="6"/>
-      <c r="X26" s="152"/>
+      <c r="X26" s="105"/>
       <c r="Y26" s="6"/>
-      <c r="Z26" s="167"/>
+      <c r="Z26" s="120"/>
       <c r="AA26" s="35"/>
       <c r="AB26" s="8"/>
       <c r="AC26" s="43"/>
@@ -3869,65 +3827,65 @@
       <c r="A27" s="33">
         <v>18</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="47"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="139"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="152"/>
+      <c r="E27" s="105"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="152"/>
+      <c r="G27" s="105"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="152"/>
+      <c r="I27" s="105"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="158"/>
+      <c r="K27" s="111"/>
       <c r="L27" s="37"/>
-      <c r="M27" s="152"/>
+      <c r="M27" s="105"/>
       <c r="N27" s="19"/>
-      <c r="O27" s="167"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="47"/>
+      <c r="O27" s="120"/>
+      <c r="P27" s="137"/>
+      <c r="Q27" s="138"/>
+      <c r="R27" s="139"/>
       <c r="S27" s="6"/>
-      <c r="T27" s="152"/>
+      <c r="T27" s="105"/>
       <c r="U27" s="6"/>
-      <c r="V27" s="152"/>
+      <c r="V27" s="105"/>
       <c r="W27" s="6"/>
-      <c r="X27" s="152"/>
+      <c r="X27" s="105"/>
       <c r="Y27" s="6"/>
-      <c r="Z27" s="167"/>
+      <c r="Z27" s="120"/>
       <c r="AA27" s="35"/>
       <c r="AB27" s="8"/>
       <c r="AC27" s="43"/>
       <c r="AD27" s="9"/>
     </row>
     <row r="28" spans="1:30" ht="42" customHeight="1">
-      <c r="A28" s="75">
+      <c r="A28" s="51">
         <v>19</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="47"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="139"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="152"/>
+      <c r="E28" s="105"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="152"/>
+      <c r="G28" s="105"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="152"/>
+      <c r="I28" s="105"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="158"/>
+      <c r="K28" s="111"/>
       <c r="L28" s="37"/>
-      <c r="M28" s="152"/>
+      <c r="M28" s="105"/>
       <c r="N28" s="19"/>
-      <c r="O28" s="167"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="47"/>
+      <c r="O28" s="120"/>
+      <c r="P28" s="137"/>
+      <c r="Q28" s="138"/>
+      <c r="R28" s="139"/>
       <c r="S28" s="6"/>
-      <c r="T28" s="152"/>
+      <c r="T28" s="105"/>
       <c r="U28" s="6"/>
-      <c r="V28" s="152"/>
+      <c r="V28" s="105"/>
       <c r="W28" s="6"/>
-      <c r="X28" s="152"/>
+      <c r="X28" s="105"/>
       <c r="Y28" s="6"/>
-      <c r="Z28" s="167"/>
+      <c r="Z28" s="120"/>
       <c r="AA28" s="35"/>
       <c r="AB28" s="8"/>
       <c r="AC28" s="43"/>
@@ -3937,31 +3895,31 @@
       <c r="A29" s="33">
         <v>20</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="47"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="139"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="152"/>
+      <c r="E29" s="105"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="152"/>
+      <c r="G29" s="105"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="152"/>
+      <c r="I29" s="105"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="158"/>
+      <c r="K29" s="111"/>
       <c r="L29" s="37"/>
-      <c r="M29" s="152"/>
+      <c r="M29" s="105"/>
       <c r="N29" s="19"/>
-      <c r="O29" s="167"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="47"/>
+      <c r="O29" s="120"/>
+      <c r="P29" s="137"/>
+      <c r="Q29" s="138"/>
+      <c r="R29" s="139"/>
       <c r="S29" s="6"/>
-      <c r="T29" s="152"/>
+      <c r="T29" s="105"/>
       <c r="U29" s="6"/>
-      <c r="V29" s="152"/>
+      <c r="V29" s="105"/>
       <c r="W29" s="6"/>
-      <c r="X29" s="152"/>
+      <c r="X29" s="105"/>
       <c r="Y29" s="6"/>
-      <c r="Z29" s="167"/>
+      <c r="Z29" s="120"/>
       <c r="AA29" s="35"/>
       <c r="AB29" s="8"/>
       <c r="AC29" s="43"/>
@@ -3971,65 +3929,65 @@
       <c r="A30" s="33">
         <v>21</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="47"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="139"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="152"/>
+      <c r="E30" s="105"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="152"/>
+      <c r="G30" s="105"/>
       <c r="H30" s="6"/>
-      <c r="I30" s="152"/>
+      <c r="I30" s="105"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="158"/>
+      <c r="K30" s="111"/>
       <c r="L30" s="37"/>
-      <c r="M30" s="152"/>
+      <c r="M30" s="105"/>
       <c r="N30" s="19"/>
-      <c r="O30" s="167"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="47"/>
+      <c r="O30" s="120"/>
+      <c r="P30" s="137"/>
+      <c r="Q30" s="138"/>
+      <c r="R30" s="139"/>
       <c r="S30" s="6"/>
-      <c r="T30" s="152"/>
+      <c r="T30" s="105"/>
       <c r="U30" s="6"/>
-      <c r="V30" s="152"/>
+      <c r="V30" s="105"/>
       <c r="W30" s="6"/>
-      <c r="X30" s="152"/>
+      <c r="X30" s="105"/>
       <c r="Y30" s="6"/>
-      <c r="Z30" s="167"/>
+      <c r="Z30" s="120"/>
       <c r="AA30" s="35"/>
       <c r="AB30" s="8"/>
       <c r="AC30" s="43"/>
       <c r="AD30" s="9"/>
     </row>
     <row r="31" spans="1:30" ht="42" customHeight="1">
-      <c r="A31" s="75">
+      <c r="A31" s="51">
         <v>22</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="47"/>
+      <c r="B31" s="137"/>
+      <c r="C31" s="139"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="152"/>
+      <c r="E31" s="105"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="152"/>
+      <c r="G31" s="105"/>
       <c r="H31" s="6"/>
-      <c r="I31" s="152"/>
+      <c r="I31" s="105"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="158"/>
+      <c r="K31" s="111"/>
       <c r="L31" s="37"/>
-      <c r="M31" s="152"/>
+      <c r="M31" s="105"/>
       <c r="N31" s="19"/>
-      <c r="O31" s="167"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="47"/>
+      <c r="O31" s="120"/>
+      <c r="P31" s="137"/>
+      <c r="Q31" s="138"/>
+      <c r="R31" s="139"/>
       <c r="S31" s="6"/>
-      <c r="T31" s="152"/>
+      <c r="T31" s="105"/>
       <c r="U31" s="6"/>
-      <c r="V31" s="152"/>
+      <c r="V31" s="105"/>
       <c r="W31" s="6"/>
-      <c r="X31" s="152"/>
+      <c r="X31" s="105"/>
       <c r="Y31" s="6"/>
-      <c r="Z31" s="167"/>
+      <c r="Z31" s="120"/>
       <c r="AA31" s="35"/>
       <c r="AB31" s="8"/>
       <c r="AC31" s="43"/>
@@ -4039,31 +3997,31 @@
       <c r="A32" s="33">
         <v>23</v>
       </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="47"/>
+      <c r="B32" s="137"/>
+      <c r="C32" s="139"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="152"/>
+      <c r="E32" s="105"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="152"/>
+      <c r="G32" s="105"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="152"/>
+      <c r="I32" s="105"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="158"/>
+      <c r="K32" s="111"/>
       <c r="L32" s="37"/>
-      <c r="M32" s="152"/>
+      <c r="M32" s="105"/>
       <c r="N32" s="19"/>
-      <c r="O32" s="167"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="47"/>
+      <c r="O32" s="120"/>
+      <c r="P32" s="137"/>
+      <c r="Q32" s="138"/>
+      <c r="R32" s="139"/>
       <c r="S32" s="6"/>
-      <c r="T32" s="152"/>
+      <c r="T32" s="105"/>
       <c r="U32" s="6"/>
-      <c r="V32" s="152"/>
+      <c r="V32" s="105"/>
       <c r="W32" s="6"/>
-      <c r="X32" s="152"/>
+      <c r="X32" s="105"/>
       <c r="Y32" s="6"/>
-      <c r="Z32" s="167"/>
+      <c r="Z32" s="120"/>
       <c r="AA32" s="35"/>
       <c r="AB32" s="8"/>
       <c r="AC32" s="43"/>
@@ -4073,65 +4031,65 @@
       <c r="A33" s="33">
         <v>24</v>
       </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="47"/>
+      <c r="B33" s="137"/>
+      <c r="C33" s="139"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="152"/>
+      <c r="E33" s="105"/>
       <c r="F33" s="6"/>
-      <c r="G33" s="152"/>
+      <c r="G33" s="105"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="152"/>
+      <c r="I33" s="105"/>
       <c r="J33" s="6"/>
-      <c r="K33" s="158"/>
+      <c r="K33" s="111"/>
       <c r="L33" s="37"/>
-      <c r="M33" s="152"/>
+      <c r="M33" s="105"/>
       <c r="N33" s="19"/>
-      <c r="O33" s="167"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="47"/>
+      <c r="O33" s="120"/>
+      <c r="P33" s="137"/>
+      <c r="Q33" s="138"/>
+      <c r="R33" s="139"/>
       <c r="S33" s="6"/>
-      <c r="T33" s="152"/>
+      <c r="T33" s="105"/>
       <c r="U33" s="6"/>
-      <c r="V33" s="152"/>
+      <c r="V33" s="105"/>
       <c r="W33" s="6"/>
-      <c r="X33" s="152"/>
+      <c r="X33" s="105"/>
       <c r="Y33" s="6"/>
-      <c r="Z33" s="167"/>
+      <c r="Z33" s="120"/>
       <c r="AA33" s="35"/>
       <c r="AB33" s="8"/>
       <c r="AC33" s="43"/>
       <c r="AD33" s="9"/>
     </row>
     <row r="34" spans="1:30" ht="42" customHeight="1">
-      <c r="A34" s="75">
+      <c r="A34" s="51">
         <v>25</v>
       </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="47"/>
+      <c r="B34" s="137"/>
+      <c r="C34" s="139"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="152"/>
+      <c r="E34" s="105"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="152"/>
+      <c r="G34" s="105"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="152"/>
+      <c r="I34" s="105"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="158"/>
+      <c r="K34" s="111"/>
       <c r="L34" s="37"/>
-      <c r="M34" s="152"/>
+      <c r="M34" s="105"/>
       <c r="N34" s="19"/>
-      <c r="O34" s="167"/>
-      <c r="P34" s="45"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="47"/>
+      <c r="O34" s="120"/>
+      <c r="P34" s="137"/>
+      <c r="Q34" s="138"/>
+      <c r="R34" s="139"/>
       <c r="S34" s="6"/>
-      <c r="T34" s="152"/>
+      <c r="T34" s="105"/>
       <c r="U34" s="6"/>
-      <c r="V34" s="152"/>
+      <c r="V34" s="105"/>
       <c r="W34" s="6"/>
-      <c r="X34" s="152"/>
+      <c r="X34" s="105"/>
       <c r="Y34" s="6"/>
-      <c r="Z34" s="167"/>
+      <c r="Z34" s="120"/>
       <c r="AA34" s="35"/>
       <c r="AB34" s="8"/>
       <c r="AC34" s="43"/>
@@ -4141,31 +4099,31 @@
       <c r="A35" s="33">
         <v>26</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="47"/>
+      <c r="B35" s="137"/>
+      <c r="C35" s="139"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="152"/>
+      <c r="E35" s="105"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="152"/>
+      <c r="G35" s="105"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="152"/>
+      <c r="I35" s="105"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="158"/>
+      <c r="K35" s="111"/>
       <c r="L35" s="37"/>
-      <c r="M35" s="152"/>
+      <c r="M35" s="105"/>
       <c r="N35" s="19"/>
-      <c r="O35" s="167"/>
-      <c r="P35" s="45"/>
-      <c r="Q35" s="46"/>
-      <c r="R35" s="47"/>
+      <c r="O35" s="120"/>
+      <c r="P35" s="137"/>
+      <c r="Q35" s="138"/>
+      <c r="R35" s="139"/>
       <c r="S35" s="6"/>
-      <c r="T35" s="152"/>
+      <c r="T35" s="105"/>
       <c r="U35" s="6"/>
-      <c r="V35" s="152"/>
+      <c r="V35" s="105"/>
       <c r="W35" s="6"/>
-      <c r="X35" s="152"/>
+      <c r="X35" s="105"/>
       <c r="Y35" s="6"/>
-      <c r="Z35" s="167"/>
+      <c r="Z35" s="120"/>
       <c r="AA35" s="35"/>
       <c r="AB35" s="8"/>
       <c r="AC35" s="43"/>
@@ -4175,65 +4133,65 @@
       <c r="A36" s="33">
         <v>27</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="47"/>
+      <c r="B36" s="137"/>
+      <c r="C36" s="139"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="152"/>
+      <c r="E36" s="105"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="152"/>
+      <c r="G36" s="105"/>
       <c r="H36" s="6"/>
-      <c r="I36" s="152"/>
+      <c r="I36" s="105"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="158"/>
+      <c r="K36" s="111"/>
       <c r="L36" s="37"/>
-      <c r="M36" s="152"/>
+      <c r="M36" s="105"/>
       <c r="N36" s="19"/>
-      <c r="O36" s="167"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="47"/>
+      <c r="O36" s="120"/>
+      <c r="P36" s="137"/>
+      <c r="Q36" s="138"/>
+      <c r="R36" s="139"/>
       <c r="S36" s="6"/>
-      <c r="T36" s="152"/>
+      <c r="T36" s="105"/>
       <c r="U36" s="6"/>
-      <c r="V36" s="152"/>
+      <c r="V36" s="105"/>
       <c r="W36" s="6"/>
-      <c r="X36" s="152"/>
+      <c r="X36" s="105"/>
       <c r="Y36" s="6"/>
-      <c r="Z36" s="167"/>
+      <c r="Z36" s="120"/>
       <c r="AA36" s="35"/>
       <c r="AB36" s="8"/>
       <c r="AC36" s="43"/>
       <c r="AD36" s="9"/>
     </row>
     <row r="37" spans="1:30" ht="42" customHeight="1">
-      <c r="A37" s="75">
+      <c r="A37" s="51">
         <v>28</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="47"/>
+      <c r="B37" s="137"/>
+      <c r="C37" s="139"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="152"/>
+      <c r="E37" s="105"/>
       <c r="F37" s="6"/>
-      <c r="G37" s="152"/>
+      <c r="G37" s="105"/>
       <c r="H37" s="6"/>
-      <c r="I37" s="152"/>
+      <c r="I37" s="105"/>
       <c r="J37" s="6"/>
-      <c r="K37" s="158"/>
+      <c r="K37" s="111"/>
       <c r="L37" s="37"/>
-      <c r="M37" s="152"/>
+      <c r="M37" s="105"/>
       <c r="N37" s="19"/>
-      <c r="O37" s="167"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="47"/>
+      <c r="O37" s="120"/>
+      <c r="P37" s="137"/>
+      <c r="Q37" s="138"/>
+      <c r="R37" s="139"/>
       <c r="S37" s="6"/>
-      <c r="T37" s="152"/>
+      <c r="T37" s="105"/>
       <c r="U37" s="6"/>
-      <c r="V37" s="152"/>
+      <c r="V37" s="105"/>
       <c r="W37" s="6"/>
-      <c r="X37" s="152"/>
+      <c r="X37" s="105"/>
       <c r="Y37" s="6"/>
-      <c r="Z37" s="167"/>
+      <c r="Z37" s="120"/>
       <c r="AA37" s="35"/>
       <c r="AB37" s="8"/>
       <c r="AC37" s="43"/>
@@ -4243,31 +4201,31 @@
       <c r="A38" s="33">
         <v>29</v>
       </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="47"/>
+      <c r="B38" s="137"/>
+      <c r="C38" s="139"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="152"/>
+      <c r="E38" s="105"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="152"/>
+      <c r="G38" s="105"/>
       <c r="H38" s="6"/>
-      <c r="I38" s="152"/>
+      <c r="I38" s="105"/>
       <c r="J38" s="6"/>
-      <c r="K38" s="158"/>
+      <c r="K38" s="111"/>
       <c r="L38" s="37"/>
-      <c r="M38" s="152"/>
+      <c r="M38" s="105"/>
       <c r="N38" s="19"/>
-      <c r="O38" s="167"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="46"/>
-      <c r="R38" s="47"/>
+      <c r="O38" s="120"/>
+      <c r="P38" s="137"/>
+      <c r="Q38" s="138"/>
+      <c r="R38" s="139"/>
       <c r="S38" s="6"/>
-      <c r="T38" s="152"/>
+      <c r="T38" s="105"/>
       <c r="U38" s="6"/>
-      <c r="V38" s="152"/>
+      <c r="V38" s="105"/>
       <c r="W38" s="6"/>
-      <c r="X38" s="152"/>
+      <c r="X38" s="105"/>
       <c r="Y38" s="6"/>
-      <c r="Z38" s="167"/>
+      <c r="Z38" s="120"/>
       <c r="AA38" s="35"/>
       <c r="AB38" s="8"/>
       <c r="AC38" s="43"/>
@@ -4277,65 +4235,65 @@
       <c r="A39" s="33">
         <v>30</v>
       </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="47"/>
+      <c r="B39" s="137"/>
+      <c r="C39" s="139"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="152"/>
+      <c r="E39" s="105"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="152"/>
+      <c r="G39" s="105"/>
       <c r="H39" s="6"/>
-      <c r="I39" s="152"/>
+      <c r="I39" s="105"/>
       <c r="J39" s="6"/>
-      <c r="K39" s="158"/>
+      <c r="K39" s="111"/>
       <c r="L39" s="37"/>
-      <c r="M39" s="152"/>
+      <c r="M39" s="105"/>
       <c r="N39" s="19"/>
-      <c r="O39" s="167"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="46"/>
-      <c r="R39" s="47"/>
+      <c r="O39" s="120"/>
+      <c r="P39" s="137"/>
+      <c r="Q39" s="138"/>
+      <c r="R39" s="139"/>
       <c r="S39" s="6"/>
-      <c r="T39" s="152"/>
+      <c r="T39" s="105"/>
       <c r="U39" s="6"/>
-      <c r="V39" s="152"/>
+      <c r="V39" s="105"/>
       <c r="W39" s="6"/>
-      <c r="X39" s="152"/>
+      <c r="X39" s="105"/>
       <c r="Y39" s="6"/>
-      <c r="Z39" s="167"/>
+      <c r="Z39" s="120"/>
       <c r="AA39" s="35"/>
       <c r="AB39" s="8"/>
       <c r="AC39" s="43"/>
       <c r="AD39" s="9"/>
     </row>
     <row r="40" spans="1:30" ht="42" customHeight="1">
-      <c r="A40" s="75">
+      <c r="A40" s="51">
         <v>31</v>
       </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="47"/>
+      <c r="B40" s="137"/>
+      <c r="C40" s="139"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="152"/>
+      <c r="E40" s="105"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="152"/>
+      <c r="G40" s="105"/>
       <c r="H40" s="6"/>
-      <c r="I40" s="152"/>
+      <c r="I40" s="105"/>
       <c r="J40" s="6"/>
-      <c r="K40" s="158"/>
+      <c r="K40" s="111"/>
       <c r="L40" s="37"/>
-      <c r="M40" s="152"/>
+      <c r="M40" s="105"/>
       <c r="N40" s="19"/>
-      <c r="O40" s="167"/>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="46"/>
-      <c r="R40" s="47"/>
+      <c r="O40" s="120"/>
+      <c r="P40" s="137"/>
+      <c r="Q40" s="138"/>
+      <c r="R40" s="139"/>
       <c r="S40" s="6"/>
-      <c r="T40" s="152"/>
+      <c r="T40" s="105"/>
       <c r="U40" s="6"/>
-      <c r="V40" s="152"/>
+      <c r="V40" s="105"/>
       <c r="W40" s="6"/>
-      <c r="X40" s="152"/>
+      <c r="X40" s="105"/>
       <c r="Y40" s="6"/>
-      <c r="Z40" s="167"/>
+      <c r="Z40" s="120"/>
       <c r="AA40" s="35"/>
       <c r="AB40" s="8"/>
       <c r="AC40" s="43"/>
@@ -4345,31 +4303,31 @@
       <c r="A41" s="33">
         <v>32</v>
       </c>
-      <c r="B41" s="45"/>
-      <c r="C41" s="47"/>
+      <c r="B41" s="137"/>
+      <c r="C41" s="139"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="152"/>
+      <c r="E41" s="105"/>
       <c r="F41" s="6"/>
-      <c r="G41" s="152"/>
+      <c r="G41" s="105"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="152"/>
+      <c r="I41" s="105"/>
       <c r="J41" s="6"/>
-      <c r="K41" s="158"/>
+      <c r="K41" s="111"/>
       <c r="L41" s="37"/>
-      <c r="M41" s="152"/>
+      <c r="M41" s="105"/>
       <c r="N41" s="19"/>
-      <c r="O41" s="167"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="46"/>
-      <c r="R41" s="47"/>
+      <c r="O41" s="120"/>
+      <c r="P41" s="137"/>
+      <c r="Q41" s="138"/>
+      <c r="R41" s="139"/>
       <c r="S41" s="6"/>
-      <c r="T41" s="152"/>
+      <c r="T41" s="105"/>
       <c r="U41" s="6"/>
-      <c r="V41" s="152"/>
+      <c r="V41" s="105"/>
       <c r="W41" s="6"/>
-      <c r="X41" s="152"/>
+      <c r="X41" s="105"/>
       <c r="Y41" s="6"/>
-      <c r="Z41" s="167"/>
+      <c r="Z41" s="120"/>
       <c r="AA41" s="35"/>
       <c r="AB41" s="8"/>
       <c r="AC41" s="43"/>
@@ -4379,65 +4337,65 @@
       <c r="A42" s="33">
         <v>33</v>
       </c>
-      <c r="B42" s="45"/>
-      <c r="C42" s="47"/>
+      <c r="B42" s="137"/>
+      <c r="C42" s="139"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="152"/>
+      <c r="E42" s="105"/>
       <c r="F42" s="6"/>
-      <c r="G42" s="152"/>
+      <c r="G42" s="105"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="152"/>
+      <c r="I42" s="105"/>
       <c r="J42" s="6"/>
-      <c r="K42" s="158"/>
+      <c r="K42" s="111"/>
       <c r="L42" s="37"/>
-      <c r="M42" s="152"/>
+      <c r="M42" s="105"/>
       <c r="N42" s="19"/>
-      <c r="O42" s="167"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="47"/>
+      <c r="O42" s="120"/>
+      <c r="P42" s="137"/>
+      <c r="Q42" s="138"/>
+      <c r="R42" s="139"/>
       <c r="S42" s="6"/>
-      <c r="T42" s="152"/>
+      <c r="T42" s="105"/>
       <c r="U42" s="6"/>
-      <c r="V42" s="152"/>
+      <c r="V42" s="105"/>
       <c r="W42" s="6"/>
-      <c r="X42" s="152"/>
+      <c r="X42" s="105"/>
       <c r="Y42" s="6"/>
-      <c r="Z42" s="167"/>
+      <c r="Z42" s="120"/>
       <c r="AA42" s="35"/>
       <c r="AB42" s="8"/>
       <c r="AC42" s="43"/>
       <c r="AD42" s="9"/>
     </row>
     <row r="43" spans="1:30" ht="42" customHeight="1">
-      <c r="A43" s="75">
+      <c r="A43" s="51">
         <v>34</v>
       </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="47"/>
+      <c r="B43" s="137"/>
+      <c r="C43" s="139"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="152"/>
+      <c r="E43" s="105"/>
       <c r="F43" s="6"/>
-      <c r="G43" s="152"/>
+      <c r="G43" s="105"/>
       <c r="H43" s="6"/>
-      <c r="I43" s="152"/>
+      <c r="I43" s="105"/>
       <c r="J43" s="6"/>
-      <c r="K43" s="158"/>
+      <c r="K43" s="111"/>
       <c r="L43" s="37"/>
-      <c r="M43" s="152"/>
+      <c r="M43" s="105"/>
       <c r="N43" s="19"/>
-      <c r="O43" s="167"/>
-      <c r="P43" s="45"/>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="47"/>
+      <c r="O43" s="120"/>
+      <c r="P43" s="137"/>
+      <c r="Q43" s="138"/>
+      <c r="R43" s="139"/>
       <c r="S43" s="6"/>
-      <c r="T43" s="152"/>
+      <c r="T43" s="105"/>
       <c r="U43" s="6"/>
-      <c r="V43" s="152"/>
+      <c r="V43" s="105"/>
       <c r="W43" s="6"/>
-      <c r="X43" s="152"/>
+      <c r="X43" s="105"/>
       <c r="Y43" s="6"/>
-      <c r="Z43" s="167"/>
+      <c r="Z43" s="120"/>
       <c r="AA43" s="35"/>
       <c r="AB43" s="8"/>
       <c r="AC43" s="43"/>
@@ -4447,31 +4405,31 @@
       <c r="A44" s="33">
         <v>35</v>
       </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="47"/>
+      <c r="B44" s="137"/>
+      <c r="C44" s="139"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="152"/>
+      <c r="E44" s="105"/>
       <c r="F44" s="6"/>
-      <c r="G44" s="152"/>
+      <c r="G44" s="105"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="152"/>
+      <c r="I44" s="105"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="158"/>
+      <c r="K44" s="111"/>
       <c r="L44" s="37"/>
-      <c r="M44" s="152"/>
+      <c r="M44" s="105"/>
       <c r="N44" s="19"/>
-      <c r="O44" s="167"/>
-      <c r="P44" s="45"/>
-      <c r="Q44" s="46"/>
-      <c r="R44" s="47"/>
+      <c r="O44" s="120"/>
+      <c r="P44" s="137"/>
+      <c r="Q44" s="138"/>
+      <c r="R44" s="139"/>
       <c r="S44" s="6"/>
-      <c r="T44" s="152"/>
+      <c r="T44" s="105"/>
       <c r="U44" s="6"/>
-      <c r="V44" s="152"/>
+      <c r="V44" s="105"/>
       <c r="W44" s="6"/>
-      <c r="X44" s="152"/>
+      <c r="X44" s="105"/>
       <c r="Y44" s="6"/>
-      <c r="Z44" s="167"/>
+      <c r="Z44" s="120"/>
       <c r="AA44" s="35"/>
       <c r="AB44" s="8"/>
       <c r="AC44" s="43"/>
@@ -4481,65 +4439,65 @@
       <c r="A45" s="33">
         <v>36</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="47"/>
+      <c r="B45" s="137"/>
+      <c r="C45" s="139"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="152"/>
+      <c r="E45" s="105"/>
       <c r="F45" s="6"/>
-      <c r="G45" s="152"/>
+      <c r="G45" s="105"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="152"/>
+      <c r="I45" s="105"/>
       <c r="J45" s="6"/>
-      <c r="K45" s="158"/>
+      <c r="K45" s="111"/>
       <c r="L45" s="37"/>
-      <c r="M45" s="152"/>
+      <c r="M45" s="105"/>
       <c r="N45" s="19"/>
-      <c r="O45" s="167"/>
-      <c r="P45" s="45"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="47"/>
+      <c r="O45" s="120"/>
+      <c r="P45" s="137"/>
+      <c r="Q45" s="138"/>
+      <c r="R45" s="139"/>
       <c r="S45" s="6"/>
-      <c r="T45" s="152"/>
+      <c r="T45" s="105"/>
       <c r="U45" s="6"/>
-      <c r="V45" s="152"/>
+      <c r="V45" s="105"/>
       <c r="W45" s="6"/>
-      <c r="X45" s="152"/>
+      <c r="X45" s="105"/>
       <c r="Y45" s="6"/>
-      <c r="Z45" s="167"/>
+      <c r="Z45" s="120"/>
       <c r="AA45" s="35"/>
       <c r="AB45" s="8"/>
       <c r="AC45" s="43"/>
       <c r="AD45" s="9"/>
     </row>
     <row r="46" spans="1:30" ht="42" customHeight="1">
-      <c r="A46" s="75">
+      <c r="A46" s="51">
         <v>37</v>
       </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="47"/>
+      <c r="B46" s="137"/>
+      <c r="C46" s="139"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="152"/>
+      <c r="E46" s="105"/>
       <c r="F46" s="6"/>
-      <c r="G46" s="152"/>
+      <c r="G46" s="105"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="152"/>
+      <c r="I46" s="105"/>
       <c r="J46" s="6"/>
-      <c r="K46" s="158"/>
+      <c r="K46" s="111"/>
       <c r="L46" s="37"/>
-      <c r="M46" s="152"/>
+      <c r="M46" s="105"/>
       <c r="N46" s="19"/>
-      <c r="O46" s="167"/>
-      <c r="P46" s="45"/>
-      <c r="Q46" s="46"/>
-      <c r="R46" s="47"/>
+      <c r="O46" s="120"/>
+      <c r="P46" s="137"/>
+      <c r="Q46" s="138"/>
+      <c r="R46" s="139"/>
       <c r="S46" s="6"/>
-      <c r="T46" s="152"/>
+      <c r="T46" s="105"/>
       <c r="U46" s="6"/>
-      <c r="V46" s="152"/>
+      <c r="V46" s="105"/>
       <c r="W46" s="6"/>
-      <c r="X46" s="152"/>
+      <c r="X46" s="105"/>
       <c r="Y46" s="6"/>
-      <c r="Z46" s="167"/>
+      <c r="Z46" s="120"/>
       <c r="AA46" s="35"/>
       <c r="AB46" s="8"/>
       <c r="AC46" s="43"/>
@@ -4549,31 +4507,31 @@
       <c r="A47" s="33">
         <v>38</v>
       </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="47"/>
+      <c r="B47" s="137"/>
+      <c r="C47" s="139"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="152"/>
+      <c r="E47" s="105"/>
       <c r="F47" s="6"/>
-      <c r="G47" s="152"/>
+      <c r="G47" s="105"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="152"/>
+      <c r="I47" s="105"/>
       <c r="J47" s="6"/>
-      <c r="K47" s="158"/>
+      <c r="K47" s="111"/>
       <c r="L47" s="37"/>
-      <c r="M47" s="152"/>
+      <c r="M47" s="105"/>
       <c r="N47" s="19"/>
-      <c r="O47" s="167"/>
-      <c r="P47" s="45"/>
-      <c r="Q47" s="46"/>
-      <c r="R47" s="47"/>
+      <c r="O47" s="120"/>
+      <c r="P47" s="137"/>
+      <c r="Q47" s="138"/>
+      <c r="R47" s="139"/>
       <c r="S47" s="6"/>
-      <c r="T47" s="152"/>
+      <c r="T47" s="105"/>
       <c r="U47" s="6"/>
-      <c r="V47" s="152"/>
+      <c r="V47" s="105"/>
       <c r="W47" s="6"/>
-      <c r="X47" s="152"/>
+      <c r="X47" s="105"/>
       <c r="Y47" s="6"/>
-      <c r="Z47" s="167"/>
+      <c r="Z47" s="120"/>
       <c r="AA47" s="35"/>
       <c r="AB47" s="8"/>
       <c r="AC47" s="43"/>
@@ -4583,31 +4541,31 @@
       <c r="A48" s="33">
         <v>39</v>
       </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="47"/>
+      <c r="B48" s="137"/>
+      <c r="C48" s="139"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="152"/>
+      <c r="E48" s="105"/>
       <c r="F48" s="6"/>
-      <c r="G48" s="152"/>
+      <c r="G48" s="105"/>
       <c r="H48" s="6"/>
-      <c r="I48" s="152"/>
+      <c r="I48" s="105"/>
       <c r="J48" s="6"/>
-      <c r="K48" s="158"/>
+      <c r="K48" s="111"/>
       <c r="L48" s="37"/>
-      <c r="M48" s="152"/>
+      <c r="M48" s="105"/>
       <c r="N48" s="19"/>
-      <c r="O48" s="167"/>
-      <c r="P48" s="45"/>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="47"/>
+      <c r="O48" s="120"/>
+      <c r="P48" s="137"/>
+      <c r="Q48" s="138"/>
+      <c r="R48" s="139"/>
       <c r="S48" s="6"/>
-      <c r="T48" s="152"/>
+      <c r="T48" s="105"/>
       <c r="U48" s="6"/>
-      <c r="V48" s="152"/>
+      <c r="V48" s="105"/>
       <c r="W48" s="6"/>
-      <c r="X48" s="152"/>
+      <c r="X48" s="105"/>
       <c r="Y48" s="6"/>
-      <c r="Z48" s="167"/>
+      <c r="Z48" s="120"/>
       <c r="AA48" s="35"/>
       <c r="AB48" s="8"/>
       <c r="AC48" s="43"/>
@@ -4617,125 +4575,104 @@
       <c r="A49" s="33">
         <v>40</v>
       </c>
-      <c r="B49" s="45"/>
-      <c r="C49" s="47"/>
+      <c r="B49" s="137"/>
+      <c r="C49" s="139"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="152"/>
+      <c r="E49" s="105"/>
       <c r="F49" s="6"/>
-      <c r="G49" s="152"/>
+      <c r="G49" s="105"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="152"/>
+      <c r="I49" s="105"/>
       <c r="J49" s="6"/>
-      <c r="K49" s="158"/>
+      <c r="K49" s="111"/>
       <c r="L49" s="37"/>
-      <c r="M49" s="152"/>
+      <c r="M49" s="105"/>
       <c r="N49" s="19"/>
-      <c r="O49" s="167"/>
-      <c r="P49" s="45"/>
-      <c r="Q49" s="46"/>
-      <c r="R49" s="47"/>
+      <c r="O49" s="120"/>
+      <c r="P49" s="137"/>
+      <c r="Q49" s="138"/>
+      <c r="R49" s="139"/>
       <c r="S49" s="6"/>
-      <c r="T49" s="152"/>
+      <c r="T49" s="105"/>
       <c r="U49" s="6"/>
-      <c r="V49" s="152"/>
+      <c r="V49" s="105"/>
       <c r="W49" s="6"/>
-      <c r="X49" s="152"/>
+      <c r="X49" s="105"/>
       <c r="Y49" s="6"/>
-      <c r="Z49" s="167"/>
+      <c r="Z49" s="120"/>
       <c r="AA49" s="35"/>
       <c r="AB49" s="8"/>
       <c r="AC49" s="43"/>
       <c r="AD49" s="9"/>
     </row>
     <row r="50" spans="1:30" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A50" s="83"/>
-      <c r="B50" s="82"/>
-      <c r="C50" s="83"/>
-      <c r="D50" s="83"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="83"/>
-      <c r="H50" s="83"/>
-      <c r="I50" s="83"/>
-      <c r="J50" s="83"/>
-      <c r="K50" s="83"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="83"/>
-      <c r="N50" s="83"/>
-      <c r="O50" s="83"/>
-      <c r="P50" s="83"/>
-      <c r="Q50" s="83"/>
-      <c r="R50" s="83"/>
-      <c r="S50" s="84" t="s">
+      <c r="A50" s="59"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="59"/>
+      <c r="J50" s="59"/>
+      <c r="K50" s="59"/>
+      <c r="L50" s="59"/>
+      <c r="M50" s="59"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="59"/>
+      <c r="P50" s="59"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="168" t="s">
         <v>5</v>
       </c>
-      <c r="T50" s="84"/>
-      <c r="U50" s="84"/>
-      <c r="V50" s="84"/>
-      <c r="W50" s="84"/>
-      <c r="X50" s="84"/>
-      <c r="Y50" s="84"/>
-      <c r="Z50" s="85"/>
+      <c r="T50" s="168"/>
+      <c r="U50" s="168"/>
+      <c r="V50" s="168"/>
+      <c r="W50" s="168"/>
+      <c r="X50" s="168"/>
+      <c r="Y50" s="168"/>
+      <c r="Z50" s="169"/>
       <c r="AA50" s="7"/>
       <c r="AB50" s="7"/>
-      <c r="AC50" s="86"/>
+      <c r="AC50" s="60"/>
     </row>
     <row r="51" spans="1:30" ht="17.25" customHeight="1">
-      <c r="A51" s="128"/>
-      <c r="B51" s="129"/>
-      <c r="C51" s="128"/>
-      <c r="D51" s="128"/>
-      <c r="E51" s="128"/>
-      <c r="F51" s="128"/>
-      <c r="G51" s="128"/>
-      <c r="H51" s="128"/>
-      <c r="I51" s="128"/>
-      <c r="J51" s="128"/>
-      <c r="K51" s="128"/>
-      <c r="L51" s="128"/>
-      <c r="M51" s="128"/>
-      <c r="N51" s="128"/>
-      <c r="O51" s="128"/>
-      <c r="P51" s="128"/>
-      <c r="Q51" s="128"/>
-      <c r="R51" s="128"/>
-      <c r="S51" s="130"/>
-      <c r="T51" s="130"/>
-      <c r="U51" s="130"/>
-      <c r="V51" s="130"/>
-      <c r="W51" s="130"/>
-      <c r="X51" s="130"/>
-      <c r="Y51" s="130"/>
-      <c r="Z51" s="130"/>
-      <c r="AA51" s="128"/>
-      <c r="AB51" s="128"/>
-      <c r="AC51" s="128"/>
+      <c r="B51" s="86"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="9"/>
+      <c r="Z51" s="9"/>
     </row>
     <row r="52" spans="1:30" ht="19.5">
-      <c r="A52" s="120"/>
-      <c r="B52" s="121"/>
+      <c r="A52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="P52" s="127" t="s">
+      <c r="P52" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="Q52" s="133" t="str">
+      <c r="Q52" s="136" t="str">
         <f>IF(Hardwarekonzept!F1="","",Hardwarekonzept!F1)</f>
         <v/>
       </c>
-      <c r="R52" s="133"/>
-      <c r="S52" s="133"/>
-      <c r="T52" s="133"/>
-      <c r="U52" s="133"/>
-      <c r="V52" s="133"/>
-      <c r="W52" s="133"/>
-      <c r="X52" s="133"/>
-      <c r="Y52" s="122" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z52" s="122"/>
-      <c r="AA52" s="122"/>
-      <c r="AB52" s="122"/>
-      <c r="AC52" s="146" t="str">
+      <c r="R52" s="136"/>
+      <c r="S52" s="136"/>
+      <c r="T52" s="136"/>
+      <c r="U52" s="136"/>
+      <c r="V52" s="136"/>
+      <c r="W52" s="136"/>
+      <c r="X52" s="136"/>
+      <c r="Y52" s="135" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z52" s="135"/>
+      <c r="AA52" s="135"/>
+      <c r="AB52" s="135"/>
+      <c r="AC52" s="99" t="str">
         <f>IF(Hardwarekonzept!C5="","",Hardwarekonzept!C5)</f>
         <v/>
       </c>
@@ -4745,86 +4682,14 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="W1:AC1"/>
-    <mergeCell ref="W3:AC3"/>
-    <mergeCell ref="Y52:AB52"/>
-    <mergeCell ref="Q52:X52"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="P36:R36"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="P39:R39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="A5:AC5"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="P49:R49"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="P43:R43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="P44:R44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="P45:R45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="P46:R46"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="S6:Z6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="S50:Z50"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="P47:R47"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:P1"/>
     <mergeCell ref="P8:Q8"/>
@@ -4836,15 +4701,87 @@
     <mergeCell ref="H3:P3"/>
     <mergeCell ref="Q1:V1"/>
     <mergeCell ref="Q3:V3"/>
+    <mergeCell ref="S6:Z6"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="P46:R46"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="P16:R16"/>
     <mergeCell ref="P42:R42"/>
-    <mergeCell ref="P47:R47"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S50:Z50"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="P39:R39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="P40:R40"/>
+    <mergeCell ref="W1:AC1"/>
+    <mergeCell ref="W3:AC3"/>
+    <mergeCell ref="Y52:AB52"/>
+    <mergeCell ref="Q52:X52"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="P36:R36"/>
+    <mergeCell ref="A5:AC5"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="P49:R49"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="P43:R43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="P44:R44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="P45:R45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A52">
@@ -4878,6 +4815,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010097CE672EB31FC448AA7E0353CA27D558" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b5a4241025f286e2d05129b61f0bfefa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2a48fa4-1071-4a1f-9232-16227662a139" xmlns:ns3="3179560c-df02-450a-821b-9e6429c13aab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0cb82ecc49fb1268e1d5b2045ebefada" ns2:_="" ns3:_="">
     <xsd:import namespace="e2a48fa4-1071-4a1f-9232-16227662a139"/>
@@ -5048,12 +4991,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5064,6 +5001,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3918046A-E928-46CD-AA27-2D6E188A5E52}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be639132-ede9-4a15-86ba-6c18882d3b83"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="931d6234-abc8-4a3c-a988-2189339a825b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AA5B2F1-0F69-42B6-BB44-ECB3031E9EBB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5082,23 +5036,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3918046A-E928-46CD-AA27-2D6E188A5E52}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be639132-ede9-4a15-86ba-6c18882d3b83"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="931d6234-abc8-4a3c-a988-2189339a825b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B163FD-8DE6-4721-9FB3-749685874232}">
   <ds:schemaRefs>

</xml_diff>